<commit_message>
Added Temperature and Ticket Features. Fixed bugs. New Line methods.
</commit_message>
<xml_diff>
--- a/Tophat-Railway/green.xlsx
+++ b/Tophat-Railway/green.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cory\git\Tophat\Tophat-Railway\src\application\TrackModel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cory\git\COE1186-TrackModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E54B83-1DDB-431F-A056-9979E9268F21}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9BE64E-E073-4332-98FA-AC290D8C4388}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{6D05A136-8A34-411F-8FBE-087023A5B490}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6D05A136-8A34-411F-8FBE-087023A5B490}"/>
   </bookViews>
   <sheets>
     <sheet name="Blocks" sheetId="1" r:id="rId1"/>
@@ -858,11 +858,11 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AA151"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E86" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R92" sqref="R92"/>
+      <selection pane="bottomRight" activeCell="J101" sqref="J101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7886,7 +7886,7 @@
         <v>3</v>
       </c>
       <c r="J101" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K101" s="5"/>
       <c r="L101" s="5">
@@ -11669,9 +11669,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R10" sqref="R10"/>
+      <selection pane="topRight" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Printing Track and Trains to the Map. Basic functionality complete.
</commit_message>
<xml_diff>
--- a/Tophat-Railway/green.xlsx
+++ b/Tophat-Railway/green.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cory\git\COE1186-TrackModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9BE64E-E073-4332-98FA-AC290D8C4388}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48542757-ECB7-4357-9F1A-75026DE79897}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6D05A136-8A34-411F-8FBE-087023A5B490}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{6D05A136-8A34-411F-8FBE-087023A5B490}"/>
   </bookViews>
   <sheets>
     <sheet name="Blocks" sheetId="1" r:id="rId1"/>
@@ -858,8 +858,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AA151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E86" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="J101" sqref="J101"/>
@@ -11669,9 +11669,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N15" sqref="N15"/>
+      <selection pane="topRight" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12235,10 +12235,10 @@
         <v>3554.92</v>
       </c>
       <c r="I16">
-        <v>-2757.05</v>
+        <v>-3121.07</v>
       </c>
       <c r="J16">
-        <v>3376.12</v>
+        <v>3436.01</v>
       </c>
       <c r="L16" t="b">
         <v>1</v>
@@ -12270,16 +12270,16 @@
         <v>97</v>
       </c>
       <c r="G17">
+        <v>-3121.07</v>
+      </c>
+      <c r="H17">
+        <v>3436.01</v>
+      </c>
+      <c r="I17">
         <v>-2757.05</v>
       </c>
-      <c r="H17">
+      <c r="J17">
         <v>3376.12</v>
-      </c>
-      <c r="I17">
-        <v>-3121.07</v>
-      </c>
-      <c r="J17">
-        <v>3436.01</v>
       </c>
       <c r="L17" t="b">
         <v>1</v>
@@ -12311,10 +12311,10 @@
         <v>100</v>
       </c>
       <c r="G18">
-        <v>-3121.07</v>
+        <v>-2757.05</v>
       </c>
       <c r="H18">
-        <v>3436.01</v>
+        <v>3376.12</v>
       </c>
       <c r="I18">
         <v>-2945.64</v>

</xml_diff>

<commit_message>
Highlighted Stations on Map. Fixed Station Names. Roman made a quick fix
</commit_message>
<xml_diff>
--- a/Tophat-Railway/green.xlsx
+++ b/Tophat-Railway/green.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cory\git\COE1186-TrackModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48542757-ECB7-4357-9F1A-75026DE79897}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5352442-DEC4-4C7E-96FE-CABEE59E6286}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{6D05A136-8A34-411F-8FBE-087023A5B490}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6D05A136-8A34-411F-8FBE-087023A5B490}"/>
   </bookViews>
   <sheets>
     <sheet name="Blocks" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="141">
   <si>
     <t>Line</t>
   </si>
@@ -223,21 +223,6 @@
   </si>
   <si>
     <t>SOUTH BANK</t>
-  </si>
-  <si>
-    <t>CENTRAL</t>
-  </si>
-  <si>
-    <t>INGLEWOOD</t>
-  </si>
-  <si>
-    <t>OVERBROOK</t>
-  </si>
-  <si>
-    <t>GLENBURY</t>
-  </si>
-  <si>
-    <t>DORMONT</t>
   </si>
   <si>
     <t>MT LEBANON</t>
@@ -442,6 +427,36 @@
   </si>
   <si>
     <t>IsClockwise</t>
+  </si>
+  <si>
+    <t>SOUTH CENTRAL</t>
+  </si>
+  <si>
+    <t>NORTH CENTRAL</t>
+  </si>
+  <si>
+    <t>SOUTH INGLEWOOD</t>
+  </si>
+  <si>
+    <t>NORTH INGLEWOOD</t>
+  </si>
+  <si>
+    <t>SOUTH OVERBROOK</t>
+  </si>
+  <si>
+    <t>NORTH OVERBROOK</t>
+  </si>
+  <si>
+    <t>WEST GLENBURY</t>
+  </si>
+  <si>
+    <t>EAST GLENBURY</t>
+  </si>
+  <si>
+    <t>NORTH DORMONT</t>
+  </si>
+  <si>
+    <t>SOUTH DORMONT</t>
   </si>
 </sst>
 </file>
@@ -858,11 +873,11 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AA151"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E95" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J101" sqref="J101"/>
+      <selection pane="bottomRight" activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -895,31 +910,31 @@
   <sheetData>
     <row r="1" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="G1" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>80</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>57</v>
@@ -937,36 +952,36 @@
         <v>58</v>
       </c>
       <c r="R1" s="10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="S1" s="10" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="T1" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y1" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z1" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="AA1" s="10" t="s">
         <v>97</v>
-      </c>
-      <c r="W1" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="X1" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="Y1" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z1" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>12</v>
@@ -1012,7 +1027,7 @@
       </c>
       <c r="R2" s="5"/>
       <c r="T2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="V2" t="b">
         <v>0</v>
@@ -1035,7 +1050,7 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>12</v>
@@ -1083,10 +1098,10 @@
         <v>59</v>
       </c>
       <c r="S3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="T3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="V3" t="b">
         <v>1</v>
@@ -1109,7 +1124,7 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>12</v>
@@ -1155,7 +1170,7 @@
       </c>
       <c r="R4" s="5"/>
       <c r="T4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="V4" t="b">
         <v>0</v>
@@ -1178,7 +1193,7 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>14</v>
@@ -1224,7 +1239,7 @@
       </c>
       <c r="R5" s="5"/>
       <c r="T5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="V5" t="b">
         <v>0</v>
@@ -1247,7 +1262,7 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>14</v>
@@ -1293,7 +1308,7 @@
       </c>
       <c r="R6" s="5"/>
       <c r="T6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="V6" t="b">
         <v>0</v>
@@ -1316,7 +1331,7 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>14</v>
@@ -1362,7 +1377,7 @@
       </c>
       <c r="R7" s="5"/>
       <c r="T7" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="V7" t="b">
         <v>0</v>
@@ -1385,7 +1400,7 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>15</v>
@@ -1431,7 +1446,7 @@
       </c>
       <c r="R8" s="7"/>
       <c r="T8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="V8" t="b">
         <v>0</v>
@@ -1454,7 +1469,7 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>15</v>
@@ -1500,7 +1515,7 @@
       </c>
       <c r="R9" s="5"/>
       <c r="T9" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="V9" t="b">
         <v>0</v>
@@ -1523,7 +1538,7 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>15</v>
@@ -1571,10 +1586,10 @@
         <v>60</v>
       </c>
       <c r="S10" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="T10" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="V10" t="b">
         <v>1</v>
@@ -1597,7 +1612,7 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>15</v>
@@ -1643,7 +1658,7 @@
       </c>
       <c r="R11" s="5"/>
       <c r="T11" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="V11" t="b">
         <v>0</v>
@@ -1666,7 +1681,7 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>15</v>
@@ -1712,7 +1727,7 @@
       </c>
       <c r="R12" s="5"/>
       <c r="T12" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="V12" t="b">
         <v>0</v>
@@ -1735,7 +1750,7 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>15</v>
@@ -1781,7 +1796,7 @@
       </c>
       <c r="R13" s="5"/>
       <c r="T13" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="V13" t="b">
         <v>0</v>
@@ -1804,7 +1819,7 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>18</v>
@@ -1850,7 +1865,7 @@
       </c>
       <c r="R14" s="5"/>
       <c r="T14" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="V14" t="b">
         <v>0</v>
@@ -1873,7 +1888,7 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>18</v>
@@ -1919,7 +1934,7 @@
       </c>
       <c r="R15" s="5"/>
       <c r="T15" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="V15" t="b">
         <v>0</v>
@@ -1942,7 +1957,7 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>18</v>
@@ -1988,7 +2003,7 @@
       </c>
       <c r="R16" s="5"/>
       <c r="T16" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="V16" t="b">
         <v>0</v>
@@ -2011,7 +2026,7 @@
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>18</v>
@@ -2059,10 +2074,10 @@
         <v>19</v>
       </c>
       <c r="S17" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="T17" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="V17" t="b">
         <v>1</v>
@@ -2085,7 +2100,7 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>20</v>
@@ -2131,7 +2146,7 @@
       </c>
       <c r="R18" s="5"/>
       <c r="T18" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="V18" t="b">
         <v>0</v>
@@ -2154,7 +2169,7 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>20</v>
@@ -2200,7 +2215,7 @@
       </c>
       <c r="R19" s="5"/>
       <c r="T19" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="V19" t="b">
         <v>0</v>
@@ -2223,7 +2238,7 @@
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>20</v>
@@ -2269,7 +2284,7 @@
       </c>
       <c r="R20" s="7"/>
       <c r="T20" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="V20" t="b">
         <v>0</v>
@@ -2292,7 +2307,7 @@
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>20</v>
@@ -2338,7 +2353,7 @@
       </c>
       <c r="R21" s="5"/>
       <c r="T21" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="V21" t="b">
         <v>0</v>
@@ -2361,7 +2376,7 @@
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>22</v>
@@ -2407,7 +2422,7 @@
       </c>
       <c r="R22" s="5"/>
       <c r="T22" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="V22" t="b">
         <v>0</v>
@@ -2430,7 +2445,7 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>22</v>
@@ -2478,10 +2493,10 @@
         <v>61</v>
       </c>
       <c r="S23" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="T23" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="V23" t="b">
         <v>1</v>
@@ -2504,7 +2519,7 @@
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>22</v>
@@ -2550,7 +2565,7 @@
       </c>
       <c r="R24" s="5"/>
       <c r="T24" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="V24" t="b">
         <v>0</v>
@@ -2573,7 +2588,7 @@
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>22</v>
@@ -2619,7 +2634,7 @@
       </c>
       <c r="R25" s="5"/>
       <c r="T25" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="V25" t="b">
         <v>0</v>
@@ -2642,7 +2657,7 @@
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>22</v>
@@ -2688,7 +2703,7 @@
       </c>
       <c r="R26" s="5"/>
       <c r="T26" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="V26" t="b">
         <v>0</v>
@@ -2711,7 +2726,7 @@
     </row>
     <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>22</v>
@@ -2757,7 +2772,7 @@
       </c>
       <c r="R27" s="5"/>
       <c r="T27" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="V27" t="b">
         <v>0</v>
@@ -2780,7 +2795,7 @@
     </row>
     <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>22</v>
@@ -2826,7 +2841,7 @@
       </c>
       <c r="R28" s="5"/>
       <c r="T28" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="V28" t="b">
         <v>0</v>
@@ -2849,7 +2864,7 @@
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>22</v>
@@ -2895,7 +2910,7 @@
       </c>
       <c r="R29" s="5"/>
       <c r="T29" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="V29" t="b">
         <v>0</v>
@@ -2918,7 +2933,7 @@
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>24</v>
@@ -2964,7 +2979,7 @@
       </c>
       <c r="R30" s="5"/>
       <c r="T30" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="V30" t="b">
         <v>0</v>
@@ -2987,7 +3002,7 @@
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>24</v>
@@ -3033,7 +3048,7 @@
       </c>
       <c r="R31" s="5"/>
       <c r="T31" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="V31" t="b">
         <v>0</v>
@@ -3056,7 +3071,7 @@
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>24</v>
@@ -3104,10 +3119,10 @@
         <v>62</v>
       </c>
       <c r="S32" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="T32" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="V32" t="b">
         <v>1</v>
@@ -3130,7 +3145,7 @@
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>24</v>
@@ -3176,7 +3191,7 @@
       </c>
       <c r="R33" s="5"/>
       <c r="T33" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="V33" t="b">
         <v>0</v>
@@ -3199,7 +3214,7 @@
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>26</v>
@@ -3245,7 +3260,7 @@
       </c>
       <c r="R34" s="5"/>
       <c r="T34" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="V34" t="b">
         <v>0</v>
@@ -3268,7 +3283,7 @@
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>26</v>
@@ -3314,7 +3329,7 @@
       </c>
       <c r="R35" s="5"/>
       <c r="T35" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="V35" t="b">
         <v>0</v>
@@ -3337,7 +3352,7 @@
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>26</v>
@@ -3383,7 +3398,7 @@
       </c>
       <c r="R36" s="5"/>
       <c r="T36" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="V36" t="b">
         <v>0</v>
@@ -3406,7 +3421,7 @@
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>27</v>
@@ -3452,7 +3467,7 @@
       </c>
       <c r="R37" s="5"/>
       <c r="T37" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V37" t="b">
         <v>0</v>
@@ -3475,7 +3490,7 @@
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>27</v>
@@ -3521,7 +3536,7 @@
       </c>
       <c r="R38" s="5"/>
       <c r="T38" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V38" t="b">
         <v>0</v>
@@ -3544,7 +3559,7 @@
     </row>
     <row r="39" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>27</v>
@@ -3590,7 +3605,7 @@
       </c>
       <c r="R39" s="5"/>
       <c r="T39" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V39" t="b">
         <v>0</v>
@@ -3611,9 +3626,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>27</v>
@@ -3658,13 +3673,13 @@
         <v>0.5</v>
       </c>
       <c r="R40" s="7" t="s">
-        <v>63</v>
+        <v>132</v>
       </c>
       <c r="S40" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="T40" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V40" t="b">
         <v>1</v>
@@ -3687,7 +3702,7 @@
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>27</v>
@@ -3733,7 +3748,7 @@
       </c>
       <c r="R41" s="5"/>
       <c r="T41" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V41" t="b">
         <v>0</v>
@@ -3756,7 +3771,7 @@
     </row>
     <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>27</v>
@@ -3802,7 +3817,7 @@
       </c>
       <c r="R42" s="5"/>
       <c r="T42" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V42" t="b">
         <v>0</v>
@@ -3825,7 +3840,7 @@
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>27</v>
@@ -3871,7 +3886,7 @@
       </c>
       <c r="R43" s="5"/>
       <c r="T43" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V43" t="b">
         <v>0</v>
@@ -3894,7 +3909,7 @@
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>27</v>
@@ -3940,7 +3955,7 @@
       </c>
       <c r="R44" s="5"/>
       <c r="T44" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V44" t="b">
         <v>0</v>
@@ -3963,7 +3978,7 @@
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>27</v>
@@ -4009,7 +4024,7 @@
       </c>
       <c r="R45" s="5"/>
       <c r="T45" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V45" t="b">
         <v>0</v>
@@ -4032,7 +4047,7 @@
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>27</v>
@@ -4078,7 +4093,7 @@
       </c>
       <c r="R46" s="5"/>
       <c r="T46" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V46" t="b">
         <v>0</v>
@@ -4101,7 +4116,7 @@
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>27</v>
@@ -4147,7 +4162,7 @@
       </c>
       <c r="R47" s="5"/>
       <c r="T47" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V47" t="b">
         <v>0</v>
@@ -4170,7 +4185,7 @@
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>27</v>
@@ -4216,7 +4231,7 @@
       </c>
       <c r="R48" s="5"/>
       <c r="T48" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V48" t="b">
         <v>0</v>
@@ -4237,9 +4252,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>27</v>
@@ -4284,13 +4299,13 @@
         <v>0.5</v>
       </c>
       <c r="R49" s="7" t="s">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="S49" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="T49" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V49" t="b">
         <v>1</v>
@@ -4313,7 +4328,7 @@
     </row>
     <row r="50" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>27</v>
@@ -4359,7 +4374,7 @@
       </c>
       <c r="R50" s="5"/>
       <c r="T50" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V50" t="b">
         <v>0</v>
@@ -4382,7 +4397,7 @@
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>27</v>
@@ -4428,7 +4443,7 @@
       </c>
       <c r="R51" s="5"/>
       <c r="T51" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V51" t="b">
         <v>0</v>
@@ -4451,7 +4466,7 @@
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>27</v>
@@ -4497,7 +4512,7 @@
       </c>
       <c r="R52" s="5"/>
       <c r="T52" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V52" t="b">
         <v>0</v>
@@ -4520,7 +4535,7 @@
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>27</v>
@@ -4566,7 +4581,7 @@
       </c>
       <c r="R53" s="5"/>
       <c r="T53" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V53" t="b">
         <v>0</v>
@@ -4589,7 +4604,7 @@
     </row>
     <row r="54" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B54" s="5" t="s">
         <v>27</v>
@@ -4635,7 +4650,7 @@
       </c>
       <c r="R54" s="5"/>
       <c r="T54" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V54" t="b">
         <v>0</v>
@@ -4658,7 +4673,7 @@
     </row>
     <row r="55" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>27</v>
@@ -4704,7 +4719,7 @@
       </c>
       <c r="R55" s="5"/>
       <c r="T55" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V55" t="b">
         <v>0</v>
@@ -4727,7 +4742,7 @@
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B56" s="5" t="s">
         <v>27</v>
@@ -4773,7 +4788,7 @@
       </c>
       <c r="R56" s="5"/>
       <c r="T56" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V56" t="b">
         <v>0</v>
@@ -4796,7 +4811,7 @@
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B57" s="5" t="s">
         <v>27</v>
@@ -4842,7 +4857,7 @@
       </c>
       <c r="R57" s="5"/>
       <c r="T57" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V57" t="b">
         <v>0</v>
@@ -4863,9 +4878,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>27</v>
@@ -4910,13 +4925,13 @@
         <v>0.5</v>
       </c>
       <c r="R58" s="7" t="s">
-        <v>65</v>
+        <v>136</v>
       </c>
       <c r="S58" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="T58" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V58" t="b">
         <v>1</v>
@@ -4939,7 +4954,7 @@
     </row>
     <row r="59" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>32</v>
@@ -4985,7 +5000,7 @@
       </c>
       <c r="R59" s="7"/>
       <c r="T59" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="V59" t="b">
         <v>0</v>
@@ -5008,7 +5023,7 @@
     </row>
     <row r="60" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>32</v>
@@ -5054,7 +5069,7 @@
       </c>
       <c r="R60" s="5"/>
       <c r="T60" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="V60" t="b">
         <v>0</v>
@@ -5077,7 +5092,7 @@
     </row>
     <row r="61" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B61" s="5" t="s">
         <v>32</v>
@@ -5123,7 +5138,7 @@
       </c>
       <c r="R61" s="5"/>
       <c r="T61" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="V61" t="b">
         <v>0</v>
@@ -5146,7 +5161,7 @@
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B62" s="5" t="s">
         <v>32</v>
@@ -5192,7 +5207,7 @@
       </c>
       <c r="R62" s="5"/>
       <c r="T62" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="V62" t="b">
         <v>0</v>
@@ -5215,7 +5230,7 @@
     </row>
     <row r="63" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B63" s="5" t="s">
         <v>32</v>
@@ -5261,7 +5276,7 @@
       </c>
       <c r="R63" s="7"/>
       <c r="T63" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="V63" t="b">
         <v>0</v>
@@ -5284,7 +5299,7 @@
     </row>
     <row r="64" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B64" s="5" t="s">
         <v>35</v>
@@ -5330,7 +5345,7 @@
       </c>
       <c r="R64" s="5"/>
       <c r="T64" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="V64" t="b">
         <v>0</v>
@@ -5353,7 +5368,7 @@
     </row>
     <row r="65" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B65" s="5" t="s">
         <v>35</v>
@@ -5399,7 +5414,7 @@
       </c>
       <c r="R65" s="5"/>
       <c r="T65" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="V65" t="b">
         <v>0</v>
@@ -5420,9 +5435,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>35</v>
@@ -5467,13 +5482,13 @@
         <v>0.5</v>
       </c>
       <c r="R66" s="7" t="s">
-        <v>66</v>
+        <v>138</v>
       </c>
       <c r="S66" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="T66" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="V66" t="b">
         <v>1</v>
@@ -5496,7 +5511,7 @@
     </row>
     <row r="67" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>35</v>
@@ -5542,7 +5557,7 @@
       </c>
       <c r="R67" s="5"/>
       <c r="T67" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="V67" t="b">
         <v>0</v>
@@ -5565,7 +5580,7 @@
     </row>
     <row r="68" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>35</v>
@@ -5611,7 +5626,7 @@
       </c>
       <c r="R68" s="5"/>
       <c r="T68" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="V68" t="b">
         <v>0</v>
@@ -5634,7 +5649,7 @@
     </row>
     <row r="69" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B69" s="5" t="s">
         <v>35</v>
@@ -5680,7 +5695,7 @@
       </c>
       <c r="R69" s="5"/>
       <c r="T69" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="V69" t="b">
         <v>0</v>
@@ -5703,7 +5718,7 @@
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B70" s="5" t="s">
         <v>37</v>
@@ -5749,7 +5764,7 @@
       </c>
       <c r="R70" s="5"/>
       <c r="T70" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="V70" t="b">
         <v>0</v>
@@ -5772,7 +5787,7 @@
     </row>
     <row r="71" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B71" s="5" t="s">
         <v>37</v>
@@ -5818,7 +5833,7 @@
       </c>
       <c r="R71" s="5"/>
       <c r="T71" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="V71" t="b">
         <v>0</v>
@@ -5841,7 +5856,7 @@
     </row>
     <row r="72" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B72" s="5" t="s">
         <v>37</v>
@@ -5887,7 +5902,7 @@
       </c>
       <c r="R72" s="5"/>
       <c r="T72" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="V72" t="b">
         <v>0</v>
@@ -5910,7 +5925,7 @@
     </row>
     <row r="73" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B73" s="5" t="s">
         <v>37</v>
@@ -5956,7 +5971,7 @@
       </c>
       <c r="R73" s="5"/>
       <c r="T73" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="V73" t="b">
         <v>0</v>
@@ -5977,9 +5992,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B74" s="5" t="s">
         <v>37</v>
@@ -6024,13 +6039,13 @@
         <v>0.5</v>
       </c>
       <c r="R74" s="7" t="s">
-        <v>67</v>
+        <v>140</v>
       </c>
       <c r="S74" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="T74" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="V74" t="b">
         <v>1</v>
@@ -6053,7 +6068,7 @@
     </row>
     <row r="75" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>39</v>
@@ -6099,7 +6114,7 @@
       </c>
       <c r="R75" s="5"/>
       <c r="T75" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V75" t="b">
         <v>0</v>
@@ -6122,7 +6137,7 @@
     </row>
     <row r="76" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>39</v>
@@ -6168,7 +6183,7 @@
       </c>
       <c r="R76" s="5"/>
       <c r="T76" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V76" t="b">
         <v>0</v>
@@ -6191,7 +6206,7 @@
     </row>
     <row r="77" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>39</v>
@@ -6237,7 +6252,7 @@
       </c>
       <c r="R77" s="5"/>
       <c r="T77" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V77" t="b">
         <v>0</v>
@@ -6260,7 +6275,7 @@
     </row>
     <row r="78" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B78" s="5" t="s">
         <v>40</v>
@@ -6305,13 +6320,13 @@
         <v>0.5</v>
       </c>
       <c r="R78" s="7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="S78" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="T78" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="V78" t="b">
         <v>1</v>
@@ -6334,7 +6349,7 @@
     </row>
     <row r="79" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>40</v>
@@ -6380,7 +6395,7 @@
       </c>
       <c r="R79" s="5"/>
       <c r="T79" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="V79" t="b">
         <v>0</v>
@@ -6403,7 +6418,7 @@
     </row>
     <row r="80" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>40</v>
@@ -6449,7 +6464,7 @@
       </c>
       <c r="R80" s="5"/>
       <c r="T80" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="V80" t="b">
         <v>0</v>
@@ -6472,7 +6487,7 @@
     </row>
     <row r="81" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B81" s="5" t="s">
         <v>40</v>
@@ -6518,7 +6533,7 @@
       </c>
       <c r="R81" s="5"/>
       <c r="T81" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="V81" t="b">
         <v>0</v>
@@ -6541,7 +6556,7 @@
     </row>
     <row r="82" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B82" s="5" t="s">
         <v>40</v>
@@ -6587,7 +6602,7 @@
       </c>
       <c r="R82" s="5"/>
       <c r="T82" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="V82" t="b">
         <v>0</v>
@@ -6610,7 +6625,7 @@
     </row>
     <row r="83" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B83" s="5" t="s">
         <v>40</v>
@@ -6656,7 +6671,7 @@
       </c>
       <c r="R83" s="5"/>
       <c r="T83" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="V83" t="b">
         <v>0</v>
@@ -6679,7 +6694,7 @@
     </row>
     <row r="84" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B84" s="5" t="s">
         <v>40</v>
@@ -6725,7 +6740,7 @@
       </c>
       <c r="R84" s="5"/>
       <c r="T84" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="V84" t="b">
         <v>0</v>
@@ -6748,7 +6763,7 @@
     </row>
     <row r="85" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B85" s="5" t="s">
         <v>40</v>
@@ -6794,7 +6809,7 @@
       </c>
       <c r="R85" s="5"/>
       <c r="T85" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="V85" t="b">
         <v>0</v>
@@ -6817,7 +6832,7 @@
     </row>
     <row r="86" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>40</v>
@@ -6863,7 +6878,7 @@
       </c>
       <c r="R86" s="5"/>
       <c r="T86" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="V86" t="b">
         <v>0</v>
@@ -6886,7 +6901,7 @@
     </row>
     <row r="87" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B87" s="5" t="s">
         <v>42</v>
@@ -6932,7 +6947,7 @@
       </c>
       <c r="R87" s="5"/>
       <c r="T87" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V87" t="b">
         <v>0</v>
@@ -6955,7 +6970,7 @@
     </row>
     <row r="88" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B88" s="5" t="s">
         <v>42</v>
@@ -7001,7 +7016,7 @@
       </c>
       <c r="R88" s="5"/>
       <c r="T88" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V88" t="b">
         <v>0</v>
@@ -7024,7 +7039,7 @@
     </row>
     <row r="89" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B89" s="5" t="s">
         <v>42</v>
@@ -7069,13 +7084,13 @@
         <v>0.5</v>
       </c>
       <c r="R89" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="S89" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="T89" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V89" t="b">
         <v>1</v>
@@ -7098,7 +7113,7 @@
     </row>
     <row r="90" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B90" s="5" t="s">
         <v>44</v>
@@ -7144,7 +7159,7 @@
       </c>
       <c r="R90" s="5"/>
       <c r="T90" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="V90" t="b">
         <v>0</v>
@@ -7167,7 +7182,7 @@
     </row>
     <row r="91" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B91" s="5" t="s">
         <v>44</v>
@@ -7213,7 +7228,7 @@
       </c>
       <c r="R91" s="5"/>
       <c r="T91" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="V91" t="b">
         <v>0</v>
@@ -7236,7 +7251,7 @@
     </row>
     <row r="92" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B92" s="5" t="s">
         <v>44</v>
@@ -7282,7 +7297,7 @@
       </c>
       <c r="R92" s="5"/>
       <c r="T92" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="V92" t="b">
         <v>0</v>
@@ -7305,7 +7320,7 @@
     </row>
     <row r="93" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B93" s="5" t="s">
         <v>44</v>
@@ -7351,7 +7366,7 @@
       </c>
       <c r="R93" s="5"/>
       <c r="T93" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="V93" t="b">
         <v>0</v>
@@ -7374,7 +7389,7 @@
     </row>
     <row r="94" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>44</v>
@@ -7420,7 +7435,7 @@
       </c>
       <c r="R94" s="5"/>
       <c r="T94" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="V94" t="b">
         <v>0</v>
@@ -7443,7 +7458,7 @@
     </row>
     <row r="95" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B95" s="5" t="s">
         <v>44</v>
@@ -7489,7 +7504,7 @@
       </c>
       <c r="R95" s="5"/>
       <c r="T95" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="V95" t="b">
         <v>0</v>
@@ -7512,7 +7527,7 @@
     </row>
     <row r="96" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B96" s="5" t="s">
         <v>44</v>
@@ -7558,7 +7573,7 @@
       </c>
       <c r="R96" s="5"/>
       <c r="T96" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="V96" t="b">
         <v>0</v>
@@ -7581,7 +7596,7 @@
     </row>
     <row r="97" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B97" s="5" t="s">
         <v>44</v>
@@ -7626,13 +7641,13 @@
         <v>0.5</v>
       </c>
       <c r="R97" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="S97" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="T97" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="V97" t="b">
         <v>1</v>
@@ -7655,7 +7670,7 @@
     </row>
     <row r="98" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B98" s="5" t="s">
         <v>44</v>
@@ -7701,7 +7716,7 @@
       </c>
       <c r="R98" s="5"/>
       <c r="T98" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="V98" t="b">
         <v>0</v>
@@ -7724,7 +7739,7 @@
     </row>
     <row r="99" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B99" s="5" t="s">
         <v>46</v>
@@ -7770,7 +7785,7 @@
       </c>
       <c r="R99" s="5"/>
       <c r="T99" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="V99" t="b">
         <v>0</v>
@@ -7793,7 +7808,7 @@
     </row>
     <row r="100" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>46</v>
@@ -7839,7 +7854,7 @@
       </c>
       <c r="R100" s="5"/>
       <c r="T100" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="V100" t="b">
         <v>0</v>
@@ -7862,7 +7877,7 @@
     </row>
     <row r="101" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>46</v>
@@ -7908,7 +7923,7 @@
       </c>
       <c r="R101" s="5"/>
       <c r="T101" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="V101" t="b">
         <v>0</v>
@@ -7931,7 +7946,7 @@
     </row>
     <row r="102" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B102" s="5" t="s">
         <v>47</v>
@@ -7977,7 +7992,7 @@
       </c>
       <c r="R102" s="5"/>
       <c r="T102" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="V102" t="b">
         <v>0</v>
@@ -8000,7 +8015,7 @@
     </row>
     <row r="103" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B103" s="5" t="s">
         <v>48</v>
@@ -8046,7 +8061,7 @@
       </c>
       <c r="R103" s="5"/>
       <c r="T103" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V103" t="b">
         <v>0</v>
@@ -8069,7 +8084,7 @@
     </row>
     <row r="104" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B104" s="5" t="s">
         <v>48</v>
@@ -8115,7 +8130,7 @@
       </c>
       <c r="R104" s="5"/>
       <c r="T104" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V104" t="b">
         <v>0</v>
@@ -8138,7 +8153,7 @@
     </row>
     <row r="105" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>48</v>
@@ -8184,7 +8199,7 @@
       </c>
       <c r="R105" s="5"/>
       <c r="T105" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="V105" t="b">
         <v>0</v>
@@ -8205,9 +8220,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B106" s="5" t="s">
         <v>49</v>
@@ -8251,15 +8266,14 @@
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
-      <c r="R106" s="7" t="str">
-        <f>R74</f>
-        <v>DORMONT</v>
+      <c r="R106" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="S106" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="T106" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="V106" t="b">
         <v>1</v>
@@ -8282,7 +8296,7 @@
     </row>
     <row r="107" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B107" s="5" t="s">
         <v>49</v>
@@ -8328,7 +8342,7 @@
       </c>
       <c r="R107" s="5"/>
       <c r="T107" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="V107" t="b">
         <v>0</v>
@@ -8351,7 +8365,7 @@
     </row>
     <row r="108" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B108" s="5" t="s">
         <v>49</v>
@@ -8397,7 +8411,7 @@
       </c>
       <c r="R108" s="5"/>
       <c r="T108" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="V108" t="b">
         <v>0</v>
@@ -8420,7 +8434,7 @@
     </row>
     <row r="109" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B109" s="5" t="s">
         <v>49</v>
@@ -8466,7 +8480,7 @@
       </c>
       <c r="R109" s="5"/>
       <c r="T109" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="V109" t="b">
         <v>0</v>
@@ -8489,7 +8503,7 @@
     </row>
     <row r="110" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B110" s="5" t="s">
         <v>49</v>
@@ -8535,7 +8549,7 @@
       </c>
       <c r="R110" s="5"/>
       <c r="T110" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="V110" t="b">
         <v>0</v>
@@ -8558,7 +8572,7 @@
     </row>
     <row r="111" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B111" s="5" t="s">
         <v>50</v>
@@ -8604,7 +8618,7 @@
       </c>
       <c r="R111" s="5"/>
       <c r="T111" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="V111" t="b">
         <v>0</v>
@@ -8627,7 +8641,7 @@
     </row>
     <row r="112" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B112" s="5" t="s">
         <v>50</v>
@@ -8673,7 +8687,7 @@
       </c>
       <c r="R112" s="5"/>
       <c r="T112" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="V112" t="b">
         <v>0</v>
@@ -8696,7 +8710,7 @@
     </row>
     <row r="113" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B113" s="5" t="s">
         <v>50</v>
@@ -8742,7 +8756,7 @@
       </c>
       <c r="R113" s="5"/>
       <c r="T113" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="V113" t="b">
         <v>0</v>
@@ -8765,7 +8779,7 @@
     </row>
     <row r="114" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B114" s="5" t="s">
         <v>50</v>
@@ -8811,7 +8825,7 @@
       </c>
       <c r="R114" s="5"/>
       <c r="T114" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="V114" t="b">
         <v>0</v>
@@ -8832,9 +8846,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B115" s="5" t="s">
         <v>50</v>
@@ -8878,15 +8892,14 @@
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
-      <c r="R115" s="7" t="str">
-        <f>R66</f>
-        <v>GLENBURY</v>
+      <c r="R115" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="S115" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="T115" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="V115" t="b">
         <v>1</v>
@@ -8909,7 +8922,7 @@
     </row>
     <row r="116" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B116" s="5" t="s">
         <v>50</v>
@@ -8955,7 +8968,7 @@
       </c>
       <c r="R116" s="5"/>
       <c r="T116" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="V116" t="b">
         <v>0</v>
@@ -8978,7 +8991,7 @@
     </row>
     <row r="117" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B117" s="5" t="s">
         <v>50</v>
@@ -9024,7 +9037,7 @@
       </c>
       <c r="R117" s="5"/>
       <c r="T117" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="V117" t="b">
         <v>0</v>
@@ -9047,7 +9060,7 @@
     </row>
     <row r="118" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B118" s="5" t="s">
         <v>51</v>
@@ -9093,7 +9106,7 @@
       </c>
       <c r="R118" s="5"/>
       <c r="T118" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="V118" t="b">
         <v>0</v>
@@ -9116,7 +9129,7 @@
     </row>
     <row r="119" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B119" s="5" t="s">
         <v>51</v>
@@ -9162,7 +9175,7 @@
       </c>
       <c r="R119" s="5"/>
       <c r="T119" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="V119" t="b">
         <v>0</v>
@@ -9185,7 +9198,7 @@
     </row>
     <row r="120" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B120" s="5" t="s">
         <v>51</v>
@@ -9231,7 +9244,7 @@
       </c>
       <c r="R120" s="5"/>
       <c r="T120" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="V120" t="b">
         <v>0</v>
@@ -9254,7 +9267,7 @@
     </row>
     <row r="121" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B121" s="5" t="s">
         <v>51</v>
@@ -9300,7 +9313,7 @@
       </c>
       <c r="R121" s="5"/>
       <c r="T121" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="V121" t="b">
         <v>0</v>
@@ -9323,7 +9336,7 @@
     </row>
     <row r="122" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B122" s="5" t="s">
         <v>51</v>
@@ -9369,7 +9382,7 @@
       </c>
       <c r="R122" s="5"/>
       <c r="T122" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="V122" t="b">
         <v>0</v>
@@ -9392,7 +9405,7 @@
     </row>
     <row r="123" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B123" s="5" t="s">
         <v>52</v>
@@ -9438,7 +9451,7 @@
       </c>
       <c r="R123" s="5"/>
       <c r="T123" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V123" t="b">
         <v>0</v>
@@ -9459,9 +9472,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B124" s="5" t="s">
         <v>52</v>
@@ -9505,15 +9518,14 @@
         <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
-      <c r="R124" s="7" t="str">
-        <f>R58</f>
-        <v>OVERBROOK</v>
+      <c r="R124" s="7" t="s">
+        <v>135</v>
       </c>
       <c r="S124" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="T124" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V124" t="b">
         <v>1</v>
@@ -9536,7 +9548,7 @@
     </row>
     <row r="125" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B125" s="5" t="s">
         <v>52</v>
@@ -9582,7 +9594,7 @@
       </c>
       <c r="R125" s="5"/>
       <c r="T125" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V125" t="b">
         <v>0</v>
@@ -9605,7 +9617,7 @@
     </row>
     <row r="126" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B126" s="5" t="s">
         <v>52</v>
@@ -9651,7 +9663,7 @@
       </c>
       <c r="R126" s="5"/>
       <c r="T126" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V126" t="b">
         <v>0</v>
@@ -9674,7 +9686,7 @@
     </row>
     <row r="127" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B127" s="5" t="s">
         <v>52</v>
@@ -9720,7 +9732,7 @@
       </c>
       <c r="R127" s="5"/>
       <c r="T127" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V127" t="b">
         <v>0</v>
@@ -9743,7 +9755,7 @@
     </row>
     <row r="128" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B128" s="5" t="s">
         <v>52</v>
@@ -9789,7 +9801,7 @@
       </c>
       <c r="R128" s="5"/>
       <c r="T128" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V128" t="b">
         <v>0</v>
@@ -9812,7 +9824,7 @@
     </row>
     <row r="129" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B129" s="5" t="s">
         <v>52</v>
@@ -9858,7 +9870,7 @@
       </c>
       <c r="R129" s="5"/>
       <c r="T129" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V129" t="b">
         <v>0</v>
@@ -9881,7 +9893,7 @@
     </row>
     <row r="130" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B130" s="5" t="s">
         <v>52</v>
@@ -9927,7 +9939,7 @@
       </c>
       <c r="R130" s="5"/>
       <c r="T130" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V130" t="b">
         <v>0</v>
@@ -9950,7 +9962,7 @@
     </row>
     <row r="131" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B131" s="5" t="s">
         <v>52</v>
@@ -9996,7 +10008,7 @@
       </c>
       <c r="R131" s="5"/>
       <c r="T131" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V131" t="b">
         <v>0</v>
@@ -10019,7 +10031,7 @@
     </row>
     <row r="132" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B132" s="5" t="s">
         <v>52</v>
@@ -10065,7 +10077,7 @@
       </c>
       <c r="R132" s="5"/>
       <c r="T132" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V132" t="b">
         <v>0</v>
@@ -10086,9 +10098,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B133" s="5" t="s">
         <v>52</v>
@@ -10132,15 +10144,14 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="R133" s="7" t="str">
-        <f>R49</f>
-        <v>INGLEWOOD</v>
+      <c r="R133" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="S133" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="T133" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V133" t="b">
         <v>1</v>
@@ -10163,7 +10174,7 @@
     </row>
     <row r="134" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B134" s="5" t="s">
         <v>52</v>
@@ -10209,7 +10220,7 @@
       </c>
       <c r="R134" s="5"/>
       <c r="T134" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V134" t="b">
         <v>0</v>
@@ -10232,7 +10243,7 @@
     </row>
     <row r="135" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B135" s="5" t="s">
         <v>52</v>
@@ -10278,7 +10289,7 @@
       </c>
       <c r="R135" s="5"/>
       <c r="T135" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V135" t="b">
         <v>0</v>
@@ -10301,7 +10312,7 @@
     </row>
     <row r="136" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B136" s="5" t="s">
         <v>52</v>
@@ -10347,7 +10358,7 @@
       </c>
       <c r="R136" s="5"/>
       <c r="T136" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V136" t="b">
         <v>0</v>
@@ -10370,7 +10381,7 @@
     </row>
     <row r="137" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B137" s="5" t="s">
         <v>52</v>
@@ -10416,7 +10427,7 @@
       </c>
       <c r="R137" s="5"/>
       <c r="T137" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V137" t="b">
         <v>0</v>
@@ -10439,7 +10450,7 @@
     </row>
     <row r="138" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B138" s="5" t="s">
         <v>52</v>
@@ -10485,7 +10496,7 @@
       </c>
       <c r="R138" s="5"/>
       <c r="T138" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V138" t="b">
         <v>0</v>
@@ -10508,7 +10519,7 @@
     </row>
     <row r="139" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B139" s="5" t="s">
         <v>52</v>
@@ -10554,7 +10565,7 @@
       </c>
       <c r="R139" s="5"/>
       <c r="T139" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V139" t="b">
         <v>0</v>
@@ -10577,7 +10588,7 @@
     </row>
     <row r="140" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B140" s="5" t="s">
         <v>52</v>
@@ -10623,7 +10634,7 @@
       </c>
       <c r="R140" s="5"/>
       <c r="T140" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V140" t="b">
         <v>0</v>
@@ -10646,7 +10657,7 @@
     </row>
     <row r="141" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B141" s="5" t="s">
         <v>52</v>
@@ -10692,7 +10703,7 @@
       </c>
       <c r="R141" s="5"/>
       <c r="T141" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V141" t="b">
         <v>0</v>
@@ -10713,9 +10724,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B142" s="5" t="s">
         <v>52</v>
@@ -10759,15 +10770,14 @@
         <f t="shared" si="9"/>
         <v>0.5</v>
       </c>
-      <c r="R142" s="7" t="str">
-        <f>R40</f>
-        <v>CENTRAL</v>
+      <c r="R142" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="S142" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="T142" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V142" t="b">
         <v>1</v>
@@ -10790,7 +10800,7 @@
     </row>
     <row r="143" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B143" s="5" t="s">
         <v>52</v>
@@ -10836,7 +10846,7 @@
       </c>
       <c r="R143" s="5"/>
       <c r="T143" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V143" t="b">
         <v>0</v>
@@ -10859,7 +10869,7 @@
     </row>
     <row r="144" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B144" s="5" t="s">
         <v>52</v>
@@ -10905,7 +10915,7 @@
       </c>
       <c r="R144" s="5"/>
       <c r="T144" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="V144" t="b">
         <v>0</v>
@@ -10928,7 +10938,7 @@
     </row>
     <row r="145" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B145" s="5" t="s">
         <v>53</v>
@@ -10974,7 +10984,7 @@
       </c>
       <c r="R145" s="5"/>
       <c r="T145" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="V145" t="b">
         <v>0</v>
@@ -10997,7 +11007,7 @@
     </row>
     <row r="146" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B146" s="5" t="s">
         <v>53</v>
@@ -11043,7 +11053,7 @@
       </c>
       <c r="R146" s="5"/>
       <c r="T146" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="V146" t="b">
         <v>0</v>
@@ -11066,7 +11076,7 @@
     </row>
     <row r="147" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B147" s="5" t="s">
         <v>53</v>
@@ -11112,7 +11122,7 @@
       </c>
       <c r="R147" s="5"/>
       <c r="T147" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="V147" t="b">
         <v>0</v>
@@ -11135,7 +11145,7 @@
     </row>
     <row r="148" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B148" s="5" t="s">
         <v>54</v>
@@ -11181,7 +11191,7 @@
       </c>
       <c r="R148" s="5"/>
       <c r="T148" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="V148" t="b">
         <v>0</v>
@@ -11204,7 +11214,7 @@
     </row>
     <row r="149" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B149" s="5" t="s">
         <v>54</v>
@@ -11251,7 +11261,7 @@
       </c>
       <c r="R149" s="5"/>
       <c r="T149" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="V149" t="b">
         <v>0</v>
@@ -11274,7 +11284,7 @@
     </row>
     <row r="150" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B150" s="5" t="s">
         <v>54</v>
@@ -11320,7 +11330,7 @@
       </c>
       <c r="R150" s="5"/>
       <c r="T150" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="V150" t="b">
         <v>0</v>
@@ -11343,7 +11353,7 @@
     </row>
     <row r="151" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B151" s="5" t="s">
         <v>55</v>
@@ -11389,7 +11399,7 @@
       </c>
       <c r="R151" s="5"/>
       <c r="T151" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="V151" t="b">
         <v>0</v>
@@ -11435,36 +11445,36 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F1" s="10"/>
       <c r="G1" s="10" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="J1" s="10"/>
       <c r="K1" s="10" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="L1" s="10" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -11669,7 +11679,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="K17" sqref="K17"/>
     </sheetView>
@@ -11685,49 +11695,49 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" t="s">
         <v>113</v>
       </c>
-      <c r="E1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H1" t="s">
-        <v>116</v>
-      </c>
-      <c r="I1" t="s">
-        <v>117</v>
-      </c>
-      <c r="J1" t="s">
-        <v>118</v>
-      </c>
       <c r="L1" s="10" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="Q1" s="10"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -11768,7 +11778,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -11809,7 +11819,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -11850,7 +11860,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
         <v>18</v>
@@ -11879,7 +11889,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
@@ -11920,7 +11930,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
@@ -11949,7 +11959,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
@@ -11978,7 +11988,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
@@ -12019,7 +12029,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
@@ -12048,7 +12058,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
         <v>32</v>
@@ -12089,7 +12099,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
         <v>35</v>
@@ -12118,7 +12128,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
@@ -12159,7 +12169,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
         <v>39</v>
@@ -12188,7 +12198,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
         <v>40</v>
@@ -12217,7 +12227,7 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
         <v>42</v>
@@ -12258,7 +12268,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
         <v>44</v>
@@ -12299,7 +12309,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B18" t="s">
         <v>46</v>
@@ -12340,7 +12350,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
         <v>47</v>
@@ -12369,7 +12379,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
         <v>48</v>
@@ -12398,7 +12408,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
         <v>49</v>
@@ -12439,7 +12449,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s">
         <v>50</v>
@@ -12468,7 +12478,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
         <v>51</v>
@@ -12509,7 +12519,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
         <v>52</v>
@@ -12538,7 +12548,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B25" t="s">
         <v>53</v>
@@ -12579,7 +12589,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
         <v>54</v>
@@ -12608,7 +12618,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
         <v>55</v>

</xml_diff>